<commit_message>
Finally optimized the cache in a great way, refactored user specific detail
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58456F6A-EB6A-4011-A2C7-C6FACC90A8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A3DAA-5B5C-4DB8-9EA7-104414AE8964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Day</t>
   </si>
@@ -83,6 +83,24 @@
   </si>
   <si>
     <t>Made chat preview and chat functionality</t>
+  </si>
+  <si>
+    <t>14/3/2024</t>
+  </si>
+  <si>
+    <t>refactored cache and Added User Basic Details Update</t>
+  </si>
+  <si>
+    <t>15/3/2024</t>
+  </si>
+  <si>
+    <t>16/3/2024</t>
+  </si>
+  <si>
+    <t>Fight with cache second level</t>
+  </si>
+  <si>
+    <t>Finally optimized the cache in a great way, refactored user specific detail</t>
   </si>
 </sst>
 </file>
@@ -431,7 +449,7 @@
   <dimension ref="A2:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -628,13 +646,55 @@
         <v>20</v>
       </c>
     </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="36" spans="3:4">
       <c r="C36" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="4">
         <f>SUM(C4:C35)</f>
-        <v>50.95</v>
+        <v>66.95</v>
       </c>
     </row>
     <row r="37" spans="3:4">

</xml_diff>

<commit_message>
Added product category and subcategory
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A3DAA-5B5C-4DB8-9EA7-104414AE8964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBB9A4-9E5D-404B-9B6E-C96FC6187795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Day</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Finally optimized the cache in a great way, refactored user specific detail</t>
+  </si>
+  <si>
+    <t>17/3/2024</t>
+  </si>
+  <si>
+    <t>Added UpdateProtectedUserDetails functionality</t>
+  </si>
+  <si>
+    <t>19/3/2024</t>
+  </si>
+  <si>
+    <t>Added Product Category and Subcategory</t>
   </si>
 </sst>
 </file>
@@ -449,7 +461,7 @@
   <dimension ref="A2:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -688,13 +700,38 @@
         <v>26</v>
       </c>
     </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="36" spans="3:4">
       <c r="C36" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="4">
         <f>SUM(C4:C35)</f>
-        <v>66.95</v>
+        <v>71.11</v>
       </c>
     </row>
     <row r="37" spans="3:4">

</xml_diff>

<commit_message>
Encrypted messages in chat
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBB9A4-9E5D-404B-9B6E-C96FC6187795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830951D5-D3E8-43BD-83D4-636F5EB6D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Day</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Added Product Category and Subcategory</t>
+  </si>
+  <si>
+    <t>20/3/2024</t>
+  </si>
+  <si>
+    <t>Encoded chat messages</t>
   </si>
 </sst>
 </file>
@@ -460,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -715,6 +721,9 @@
       </c>
     </row>
     <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
@@ -723,6 +732,20 @@
       </c>
       <c r="D20" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="3:4">
@@ -731,7 +754,7 @@
       </c>
       <c r="D36" s="4">
         <f>SUM(C4:C35)</f>
-        <v>71.11</v>
+        <v>111.11</v>
       </c>
     </row>
     <row r="37" spans="3:4">

</xml_diff>

<commit_message>
made search engine functionality better
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830951D5-D3E8-43BD-83D4-636F5EB6D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80782428-4600-4E2C-9DF9-3D7D8DC73B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Encoded chat messages</t>
+  </si>
+  <si>
+    <t>21/3/2024</t>
+  </si>
+  <si>
+    <t>Added search engine functionality for products</t>
   </si>
 </sst>
 </file>
@@ -466,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -742,10 +748,24 @@
         <v>31</v>
       </c>
       <c r="C21" s="1">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="3:4">
@@ -754,7 +774,7 @@
       </c>
       <c r="D36" s="4">
         <f>SUM(C4:C35)</f>
-        <v>111.11</v>
+        <v>83.11</v>
       </c>
     </row>
     <row r="37" spans="3:4">

</xml_diff>

<commit_message>
Refactored search functionality, a lot of features added (category search, etc)
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80782428-4600-4E2C-9DF9-3D7D8DC73B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48257C77-0DAC-4797-BDC5-8853D1ED3CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Day</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Added search engine functionality for products</t>
+  </si>
+  <si>
+    <t>22/3/2024</t>
+  </si>
+  <si>
+    <t>Refactored search functionality, a lot of features added (category search, etc)</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
   <dimension ref="A2:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -768,13 +774,27 @@
         <v>34</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="36" spans="3:4">
       <c r="C36" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="4">
         <f>SUM(C4:C35)</f>
-        <v>83.11</v>
+        <v>89.61</v>
       </c>
     </row>
     <row r="37" spans="3:4">

</xml_diff>

<commit_message>
Refactored search call method
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5890D342-E5FD-4C28-970D-8CAB777F65B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D95C81-05C9-4FCA-97D0-87CEEFDA3879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Day</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Improved security a lot</t>
+  </si>
+  <si>
+    <t>Refactored search call method</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -975,9 +978,15 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="B34" s="2">
+        <v>45355</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1"/>
@@ -997,7 +1006,7 @@
       </c>
       <c r="D39" s="4">
         <f>SUM(C4:C38)</f>
-        <v>135.81</v>
+        <v>137.31</v>
       </c>
     </row>
     <row r="40" spans="1:4">

</xml_diff>

<commit_message>
Configured correctly oath2 flow
</commit_message>
<xml_diff>
--- a/files/documentation/ProjectTimeline.xlsx
+++ b/files/documentation/ProjectTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0BD829-916E-4E2F-B43E-2D4D4E617F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268755D3-D3BD-4ADF-AA0A-A800D65FA8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Day</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Added User Ban and removed cron job ms, will have cron on each microservice</t>
+  </si>
+  <si>
+    <t>Configured correctly Oauth2 flow</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D39" sqref="D39:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1005,9 +1008,15 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="B36" s="2">
+        <v>45416</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
       <c r="C39" s="4" t="s">
@@ -1015,7 +1024,7 @@
       </c>
       <c r="D39" s="4">
         <f>SUM(C4:C38)</f>
-        <v>142.31</v>
+        <v>146.81</v>
       </c>
     </row>
     <row r="40" spans="1:4">

</xml_diff>